<commit_message>
API Fluent Entities Config Part 1
</commit_message>
<xml_diff>
--- a/Documents/DatabaseTemplate.xlsx
+++ b/Documents/DatabaseTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ZiTechDev\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC733B1-1CCA-4AFE-9505-522B866D4F4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C218C4EC-470C-4258-8398-9A3D97A73834}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="66">
   <si>
     <t>Users</t>
   </si>
@@ -36,12 +36,6 @@
     <t>UserRole</t>
   </si>
   <si>
-    <t>Permission</t>
-  </si>
-  <si>
-    <t>Actions</t>
-  </si>
-  <si>
     <t>Functions</t>
   </si>
   <si>
@@ -111,18 +105,12 @@
     <t>RoleId</t>
   </si>
   <si>
-    <t>permission</t>
-  </si>
-  <si>
     <t>FunctionId</t>
   </si>
   <si>
     <t>Desciption</t>
   </si>
   <si>
-    <t>actions</t>
-  </si>
-  <si>
     <t>functions</t>
   </si>
   <si>
@@ -177,9 +165,6 @@
     <t>categories</t>
   </si>
   <si>
-    <t>Desciptions</t>
-  </si>
-  <si>
     <t>SEODescription</t>
   </si>
   <si>
@@ -219,20 +204,32 @@
     <t>LanguageId</t>
   </si>
   <si>
-    <t>ActionName</t>
-  </si>
-  <si>
     <t>ActionTime</t>
   </si>
   <si>
     <t>Thumbnail</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>activities</t>
+  </si>
+  <si>
+    <t>Activities</t>
+  </si>
+  <si>
+    <t>Permissions</t>
+  </si>
+  <si>
+    <t>permissions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,6 +254,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -278,10 +291,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,7 +614,7 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15:I22"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -608,7 +623,8 @@
     <col min="2" max="2" width="29.59765625" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="7" width="10.796875" customWidth="1"/>
+    <col min="6" max="6" width="10.796875" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="15.3984375" customWidth="1"/>
     <col min="9" max="9" width="13.796875" customWidth="1"/>
     <col min="10" max="10" width="14.5" customWidth="1"/>
@@ -619,28 +635,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -653,28 +669,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>27</v>
+        <v>11</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -682,274 +698,281 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>33</v>
+        <v>22</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D8" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D10" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D16" s="2" t="s">
-        <v>35</v>
+      <c r="D16" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>55</v>
+        <v>37</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>55</v>
+        <v>21</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="H17" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="E18" s="2" t="s">
-        <v>26</v>
+      <c r="E18" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E19" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E20" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E21" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E22" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="E23" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>63</v>
+      <c r="E23" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E24" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D27" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -960,22 +983,22 @@
     </row>
     <row r="28" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D28" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D29" s="2" t="s">
-        <v>64</v>
+      <c r="D29" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D30" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D31" s="2" t="s">
-        <v>26</v>
+      <c r="D31" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fluent API Configuration Part 2
</commit_message>
<xml_diff>
--- a/Documents/DatabaseTemplate.xlsx
+++ b/Documents/DatabaseTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ZiTechDev\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C218C4EC-470C-4258-8398-9A3D97A73834}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441F30C5-29CC-44C6-A621-0ECC51B3B351}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
   </bookViews>
@@ -123,9 +123,6 @@
     <t>ParentId</t>
   </si>
   <si>
-    <t>configurations</t>
-  </si>
-  <si>
     <t>key</t>
   </si>
   <si>
@@ -223,6 +220,9 @@
   </si>
   <si>
     <t>permissions</t>
+  </si>
+  <si>
+    <t>settings</t>
   </si>
 </sst>
 </file>
@@ -271,12 +271,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -291,12 +297,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,7 +621,7 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -647,16 +654,16 @@
         <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -690,7 +697,7 @@
         <v>11</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -698,7 +705,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
@@ -719,12 +726,12 @@
         <v>21</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>13</v>
@@ -742,12 +749,12 @@
         <v>22</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>14</v>
@@ -810,29 +817,29 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H14" s="1" t="s">
+      <c r="D14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>11</v>
@@ -858,36 +865,36 @@
         <v>31</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E17" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="4:10" x14ac:dyDescent="0.25">
@@ -895,7 +902,7 @@
         <v>24</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>22</v>
@@ -906,73 +913,73 @@
     </row>
     <row r="19" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E19" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>31</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E20" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E21" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E22" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E23" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E24" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D27" s="1" t="s">
-        <v>56</v>
+      <c r="D27" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -993,7 +1000,7 @@
     </row>
     <row r="30" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D30" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="4:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Data Seeding Part 1
</commit_message>
<xml_diff>
--- a/Documents/DatabaseTemplate.xlsx
+++ b/Documents/DatabaseTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ZiTechDev\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66677ABD-1D01-401B-A1D8-D59575ACD63A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E4F5BF-3F0F-4C9D-B074-43C598B98610}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="68">
   <si>
     <t>Users</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Functions</t>
   </si>
   <si>
-    <t>Configurations</t>
-  </si>
-  <si>
     <t>Categories</t>
   </si>
   <si>
@@ -120,18 +117,9 @@
     <t>ParentId</t>
   </si>
   <si>
-    <t>key</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
     <t>posts</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
     <t>CreatedDate</t>
   </si>
   <si>
@@ -229,6 +217,18 @@
   </si>
   <si>
     <t>LastName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Settings</t>
   </si>
 </sst>
 </file>
@@ -401,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -421,6 +421,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,7 +739,7 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18:J19"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -759,28 +760,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -793,28 +794,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -822,71 +823,68 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>66</v>
-      </c>
       <c r="E4" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="I4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="14"/>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="I5" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -894,20 +892,20 @@
         <v>3</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="14"/>
       <c r="H6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="14"/>
@@ -915,214 +913,211 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D8" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D9" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D10" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D14" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D16" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E17" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="I17" s="2"/>
     </row>
     <row r="18" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E18" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>21</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E19" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E20" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E21" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E22" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>56</v>
+        <v>37</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E23" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>56</v>
+        <v>38</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="4:10" x14ac:dyDescent="0.25">
       <c r="E24" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D27" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -1133,22 +1128,22 @@
     </row>
     <row r="28" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D28" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D29" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D30" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D31" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data Seeding Part 2
</commit_message>
<xml_diff>
--- a/Documents/DatabaseTemplate.xlsx
+++ b/Documents/DatabaseTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ZiTechDev\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E4F5BF-3F0F-4C9D-B074-43C598B98610}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8CF028-D9D5-4633-AFDA-89ABF660CAF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="73">
   <si>
     <t>Users</t>
   </si>
@@ -229,6 +229,21 @@
   </si>
   <si>
     <t>Settings</t>
+  </si>
+  <si>
+    <t>images</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Caption</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>EncodeString</t>
   </si>
 </sst>
 </file>
@@ -309,7 +324,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -317,111 +332,24 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -736,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A2CE64-A3F4-45CE-9B61-6335E4BCB128}">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -753,6 +681,7 @@
     <col min="8" max="8" width="15.3984375" customWidth="1"/>
     <col min="9" max="9" width="13.796875" customWidth="1"/>
     <col min="10" max="10" width="14.5" customWidth="1"/>
+    <col min="11" max="11" width="12.8984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -762,16 +691,16 @@
       <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>59</v>
       </c>
       <c r="H1" s="4" t="s">
@@ -783,7 +712,9 @@
       <c r="J1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="1"/>
+      <c r="K1" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -796,17 +727,17 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
+      <c r="G2" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>10</v>
@@ -816,6 +747,9 @@
       </c>
       <c r="J2" s="2" t="s">
         <v>65</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -825,17 +759,17 @@
       <c r="B3" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>23</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>19</v>
@@ -845,22 +779,22 @@
       </c>
       <c r="J3" s="2" t="s">
         <v>66</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="F4" s="8"/>
       <c r="H4" s="2" t="s">
         <v>25</v>
       </c>
@@ -869,17 +803,20 @@
       </c>
       <c r="J4" s="2" t="s">
         <v>55</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="14"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
       <c r="H5" s="2" t="s">
         <v>28</v>
       </c>
@@ -891,11 +828,11 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="14"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
       <c r="H6" s="3" t="s">
         <v>29</v>
       </c>
@@ -904,59 +841,59 @@
       <c r="A7" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="14"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="14"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="14"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="14"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="14"/>
-    </row>
-    <row r="12" spans="1:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="17"/>
-      <c r="F12" s="18"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="12" t="s">
         <v>64</v>
       </c>
     </row>
@@ -980,6 +917,9 @@
         <v>48</v>
       </c>
       <c r="J14" s="1"/>
+      <c r="K14" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -1003,6 +943,9 @@
       <c r="I15" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="K15" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D16" s="3" t="s">
@@ -1023,8 +966,11 @@
       <c r="I16" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E17" s="2" t="s">
         <v>46</v>
       </c>
@@ -1037,19 +983,31 @@
       <c r="H17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="I17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E18" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="H18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E19" s="2" t="s">
         <v>32</v>
       </c>
@@ -1057,13 +1015,16 @@
         <v>29</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="4:10" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E20" s="2" t="s">
         <v>33</v>
       </c>
@@ -1071,54 +1032,42 @@
         <v>33</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="4:10" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E21" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="H21" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E22" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H22" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="4:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E23" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I23" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="4:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E24" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D27" s="4" t="s">
-        <v>50</v>
-      </c>
+    <row r="27" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -1126,26 +1075,6 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D28" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D29" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D30" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D31" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Create Business Structure And Complete Activity Business
</commit_message>
<xml_diff>
--- a/Documents/DatabaseTemplate.xlsx
+++ b/Documents/DatabaseTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ZiTechDev\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3560DF44-7189-4906-AFC3-7D8287FAC936}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9D9406-197E-42BE-9031-D7BF2E987CD3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
   </bookViews>
@@ -664,7 +664,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fix PostGallery Attributes Fix Spell SortedOrder to SortOder Fix Delete Default Enum to Use Boolean Fix Add Gender in AppUser Fix Add GenderType to Enum Re-Migration
</commit_message>
<xml_diff>
--- a/Documents/DatabaseTemplate.xlsx
+++ b/Documents/DatabaseTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ZiTechDev\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3560DF44-7189-4906-AFC3-7D8287FAC936}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9D9406-197E-42BE-9031-D7BF2E987CD3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
   </bookViews>
@@ -664,7 +664,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Role site Role assign Reset password Copy Id js
</commit_message>
<xml_diff>
--- a/Documents/DatabaseTemplate.xlsx
+++ b/Documents/DatabaseTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ZiTechDev\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA995C9-70C6-4B07-8E3F-20523285BF95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086C21EF-976E-4E56-BACD-8997F40B9246}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="77">
   <si>
     <t>Users</t>
   </si>
@@ -250,6 +250,12 @@
   </si>
   <si>
     <t>Gender</t>
+  </si>
+  <si>
+    <t>Avatar</t>
+  </si>
+  <si>
+    <t>Background</t>
   </si>
 </sst>
 </file>
@@ -681,7 +687,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="M14" sqref="M14:M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -920,11 +926,18 @@
       <c r="B15" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="13"/>
+      <c r="D15" s="12" t="s">
+        <v>75</v>
+      </c>
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D16" s="12" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D17" s="4" t="s">

</xml_diff>

<commit_message>
[Successfully build but not test yet] Profile Refactor Region Code LockOut Email refactor to api layer again
</commit_message>
<xml_diff>
--- a/Documents/DatabaseTemplate.xlsx
+++ b/Documents/DatabaseTemplate.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ZiTechDev\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086C21EF-976E-4E56-BACD-8997F40B9246}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06823B8D-15D6-4C5C-AFA4-3CDFAA64ADD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12504" activeTab="1" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,8 +25,52 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Hiếu Nguyễn Ngọc</author>
+  </authors>
+  <commentList>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{C8AAB5A6-A565-4796-8018-8E8781D46AD6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hiếu Nguyễn Ngọc:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+FirstName
+MiddleName
+LastName
+UserName
+DisplayName
+DateOfBirth
+Gender
+PhoneNumber
+Email
+Password (auto generation)
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="104">
   <si>
     <t>Users</t>
   </si>
@@ -256,13 +301,95 @@
   </si>
   <si>
     <t>Background</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Auth</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>ForgotPassword</t>
+  </si>
+  <si>
+    <t>ConfirmEmail</t>
+  </si>
+  <si>
+    <t>ConfirmPhone</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>ResetPassword</t>
+  </si>
+  <si>
+    <t>GetProfile</t>
+  </si>
+  <si>
+    <t>EditProfile</t>
+  </si>
+  <si>
+    <t>ChangePassword</t>
+  </si>
+  <si>
+    <t>ChangeEmail</t>
+  </si>
+  <si>
+    <t>ChangePhone</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>RegisterRequest</t>
+  </si>
+  <si>
+    <t>ResetPasswordRequest</t>
+  </si>
+  <si>
+    <t>LoginRequest</t>
+  </si>
+  <si>
+    <t>ForgotPasswordRequest</t>
+  </si>
+  <si>
+    <t>UserViewModel</t>
+  </si>
+  <si>
+    <t>EditProfileRequest</t>
+  </si>
+  <si>
+    <t>ChangePasswordRequest</t>
+  </si>
+  <si>
+    <t>ChangeEmailRequest</t>
+  </si>
+  <si>
+    <t>ChangePhoneRequest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,6 +429,19 @@
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -354,7 +494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -370,6 +510,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A2CE64-A3F4-45CE-9B61-6335E4BCB128}">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14:M22"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1128,4 +1275,135 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD12C05A-8E81-4663-8687-3246FBF4929F}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.3984375" style="16" customWidth="1"/>
+    <col min="2" max="2" width="17.59765625" customWidth="1"/>
+    <col min="3" max="3" width="24.8984375" customWidth="1"/>
+    <col min="4" max="4" width="31.5" customWidth="1"/>
+    <col min="5" max="5" width="18.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>